<commit_message>
update v0.7.1 IG with new value sets
</commit_message>
<xml_diff>
--- a/v0.7.1/StructureDefinition-Communication.xlsx
+++ b/v0.7.1/StructureDefinition-Communication.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="297">
   <si>
     <t>Property</t>
   </si>
@@ -238,6 +238,10 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
   <si>
     <t>A record of information transmitted from a sender to a receiver</t>
@@ -1425,10 +1429,10 @@
         <v>72</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M2" t="s" s="2">
         <v>19</v>
@@ -1497,21 +1501,21 @@
         <v>72</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AL2" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AM2" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
@@ -1522,7 +1526,7 @@
         <v>73</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s" s="2">
         <v>72</v>
@@ -1531,19 +1535,19 @@
         <v>72</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N3" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
@@ -1593,13 +1597,13 @@
         <v>72</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI3" t="s" s="2">
         <v>72</v>
@@ -1619,10 +1623,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
@@ -1633,7 +1637,7 @@
         <v>73</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>72</v>
@@ -1642,16 +1646,16 @@
         <v>72</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1702,19 +1706,19 @@
         <v>72</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI4" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK4" t="s" s="2">
         <v>72</v>
@@ -1728,10 +1732,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -1742,28 +1746,28 @@
         <v>73</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>72</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N5" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
@@ -1813,19 +1817,19 @@
         <v>72</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI5" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK5" t="s" s="2">
         <v>72</v>
@@ -1839,10 +1843,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -1853,7 +1857,7 @@
         <v>73</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s" s="2">
         <v>72</v>
@@ -1865,16 +1869,16 @@
         <v>72</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N6" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
@@ -1900,13 +1904,13 @@
         <v>72</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AA6" t="s" s="2">
         <v>72</v>
@@ -1924,19 +1928,19 @@
         <v>72</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI6" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK6" t="s" s="2">
         <v>72</v>
@@ -1950,21 +1954,21 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
         <v>73</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s" s="2">
         <v>72</v>
@@ -1976,16 +1980,16 @@
         <v>72</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N7" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
@@ -2035,19 +2039,19 @@
         <v>72</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI7" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK7" t="s" s="2">
         <v>72</v>
@@ -2056,19 +2060,19 @@
         <v>72</v>
       </c>
       <c r="AM7" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
@@ -2087,16 +2091,16 @@
         <v>72</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N8" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -2146,7 +2150,7 @@
         <v>72</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>73</v>
@@ -2167,19 +2171,19 @@
         <v>72</v>
       </c>
       <c r="AM8" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
@@ -2198,16 +2202,16 @@
         <v>72</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N9" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
@@ -2257,7 +2261,7 @@
         <v>72</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>73</v>
@@ -2269,7 +2273,7 @@
         <v>72</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AK9" t="s" s="2">
         <v>72</v>
@@ -2278,19 +2282,19 @@
         <v>72</v>
       </c>
       <c r="AM9" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
@@ -2303,25 +2307,25 @@
         <v>72</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J10" t="s" s="2">
         <v>72</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O10" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="P10" t="s" s="2">
         <v>72</v>
@@ -2370,7 +2374,7 @@
         <v>72</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>73</v>
@@ -2382,7 +2386,7 @@
         <v>72</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AK10" t="s" s="2">
         <v>72</v>
@@ -2391,15 +2395,15 @@
         <v>72</v>
       </c>
       <c r="AM10" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2407,7 +2411,7 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G11" t="s" s="2">
         <v>74</v>
@@ -2419,22 +2423,22 @@
         <v>72</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O11" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P11" t="s" s="2">
         <v>72</v>
@@ -2483,7 +2487,7 @@
         <v>72</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>73</v>
@@ -2495,13 +2499,13 @@
         <v>72</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AM11" t="s" s="2">
         <v>72</v>
@@ -2509,10 +2513,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2532,16 +2536,16 @@
         <v>72</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -2592,7 +2596,7 @@
         <v>72</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>73</v>
@@ -2604,24 +2608,24 @@
         <v>72</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AL12" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -2641,19 +2645,19 @@
         <v>72</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
@@ -2703,7 +2707,7 @@
         <v>72</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>73</v>
@@ -2715,28 +2719,28 @@
         <v>72</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
@@ -2752,19 +2756,19 @@
         <v>72</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" t="s" s="2">
@@ -2814,7 +2818,7 @@
         <v>72</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>73</v>
@@ -2826,10 +2830,10 @@
         <v>72</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>72</v>
@@ -2840,14 +2844,14 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
@@ -2863,16 +2867,16 @@
         <v>72</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -2923,7 +2927,7 @@
         <v>72</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>73</v>
@@ -2935,10 +2939,10 @@
         <v>72</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>72</v>
@@ -2949,10 +2953,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -2975,13 +2979,13 @@
         <v>72</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -3032,7 +3036,7 @@
         <v>72</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>73</v>
@@ -3044,7 +3048,7 @@
         <v>72</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>72</v>
@@ -3058,10 +3062,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3069,31 +3073,31 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>72</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" t="s" s="2">
@@ -3119,13 +3123,13 @@
         <v>72</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Z17" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>72</v>
@@ -3143,25 +3147,25 @@
         <v>72</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI17" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="AM17" t="s" s="2">
         <v>72</v>
@@ -3169,21 +3173,21 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
         <v>73</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>72</v>
@@ -3192,19 +3196,19 @@
         <v>72</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
@@ -3230,13 +3234,13 @@
         <v>72</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="Z18" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AA18" t="s" s="2">
         <v>72</v>
@@ -3254,22 +3258,22 @@
         <v>72</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI18" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>72</v>
@@ -3280,10 +3284,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3306,16 +3310,16 @@
         <v>72</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
@@ -3341,13 +3345,13 @@
         <v>72</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Z19" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AA19" t="s" s="2">
         <v>72</v>
@@ -3365,7 +3369,7 @@
         <v>72</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>73</v>
@@ -3377,13 +3381,13 @@
         <v>72</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AM19" t="s" s="2">
         <v>72</v>
@@ -3391,10 +3395,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3405,7 +3409,7 @@
         <v>73</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>72</v>
@@ -3414,26 +3418,26 @@
         <v>72</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
         <v>72</v>
       </c>
       <c r="Q20" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="R20" t="s" s="2">
         <v>72</v>
@@ -3454,13 +3458,13 @@
         <v>72</v>
       </c>
       <c r="X20" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Y20" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="Z20" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AA20" t="s" s="2">
         <v>72</v>
@@ -3478,25 +3482,25 @@
         <v>72</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI20" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>72</v>
@@ -3504,10 +3508,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3530,13 +3534,13 @@
         <v>72</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -3563,13 +3567,13 @@
         <v>72</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Z21" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AA21" t="s" s="2">
         <v>72</v>
@@ -3587,7 +3591,7 @@
         <v>72</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>73</v>
@@ -3599,7 +3603,7 @@
         <v>72</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>72</v>
@@ -3613,21 +3617,21 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
         <v>73</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>72</v>
@@ -3636,16 +3640,16 @@
         <v>72</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -3696,25 +3700,25 @@
         <v>72</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>72</v>
@@ -3722,10 +3726,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -3736,7 +3740,7 @@
         <v>73</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>72</v>
@@ -3748,16 +3752,16 @@
         <v>72</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
@@ -3783,13 +3787,13 @@
         <v>72</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="Z23" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>72</v>
@@ -3807,25 +3811,25 @@
         <v>72</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>72</v>
@@ -3833,10 +3837,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -3859,16 +3863,16 @@
         <v>72</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
@@ -3918,7 +3922,7 @@
         <v>72</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>73</v>
@@ -3930,13 +3934,13 @@
         <v>72</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>72</v>
@@ -3944,10 +3948,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -3958,7 +3962,7 @@
         <v>73</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>72</v>
@@ -3967,19 +3971,19 @@
         <v>72</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
@@ -4029,25 +4033,25 @@
         <v>72</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>72</v>
@@ -4055,10 +4059,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4069,7 +4073,7 @@
         <v>73</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>72</v>
@@ -4081,13 +4085,13 @@
         <v>72</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -4138,25 +4142,25 @@
         <v>72</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>72</v>
@@ -4164,10 +4168,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4178,7 +4182,7 @@
         <v>73</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>72</v>
@@ -4190,13 +4194,13 @@
         <v>72</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -4247,25 +4251,25 @@
         <v>72</v>
       </c>
       <c r="AF27" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AG27" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AH27" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI27" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AJ27" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AK27" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="AL27" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AG27" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH27" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI27" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AJ27" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AK27" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="AL27" t="s" s="2">
-        <v>239</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>72</v>
@@ -4273,10 +4277,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4299,13 +4303,13 @@
         <v>72</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -4356,7 +4360,7 @@
         <v>72</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>73</v>
@@ -4368,13 +4372,13 @@
         <v>72</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>72</v>
@@ -4382,10 +4386,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4396,7 +4400,7 @@
         <v>73</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>72</v>
@@ -4408,13 +4412,13 @@
         <v>72</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -4465,25 +4469,25 @@
         <v>72</v>
       </c>
       <c r="AF29" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AK29" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="AL29" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="AL29" t="s" s="2">
-        <v>249</v>
       </c>
       <c r="AM29" t="s" s="2">
         <v>72</v>
@@ -4491,10 +4495,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4514,19 +4518,19 @@
         <v>72</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -4552,13 +4556,13 @@
         <v>72</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Z30" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>72</v>
@@ -4576,7 +4580,7 @@
         <v>72</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>73</v>
@@ -4588,24 +4592,24 @@
         <v>72</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -4625,16 +4629,16 @@
         <v>72</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -4685,7 +4689,7 @@
         <v>72</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>73</v>
@@ -4697,24 +4701,24 @@
         <v>72</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -4737,13 +4741,13 @@
         <v>72</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -4794,7 +4798,7 @@
         <v>72</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>73</v>
@@ -4806,7 +4810,7 @@
         <v>72</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>72</v>
@@ -4820,10 +4824,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -4834,7 +4838,7 @@
         <v>73</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>72</v>
@@ -4846,13 +4850,13 @@
         <v>72</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -4903,13 +4907,13 @@
         <v>72</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>73</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>72</v>
@@ -4924,19 +4928,19 @@
         <v>72</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
@@ -4955,16 +4959,16 @@
         <v>72</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
@@ -5014,7 +5018,7 @@
         <v>72</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>73</v>
@@ -5026,7 +5030,7 @@
         <v>72</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>72</v>
@@ -5035,19 +5039,19 @@
         <v>72</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5060,25 +5064,25 @@
         <v>72</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O35" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="P35" t="s" s="2">
         <v>72</v>
@@ -5127,7 +5131,7 @@
         <v>72</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>73</v>
@@ -5139,7 +5143,7 @@
         <v>72</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>72</v>
@@ -5148,15 +5152,15 @@
         <v>72</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5164,10 +5168,10 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>72</v>
@@ -5179,13 +5183,13 @@
         <v>72</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -5236,19 +5240,19 @@
         <v>72</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>72</v>
@@ -5262,10 +5266,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5288,13 +5292,13 @@
         <v>72</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5345,7 +5349,7 @@
         <v>72</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>73</v>
@@ -5357,10 +5361,10 @@
         <v>72</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>72</v>

</xml_diff>